<commit_message>
Fini : -menu des stats de blocks
</commit_message>
<xml_diff>
--- a/Reward bouillancube.xlsx
+++ b/Reward bouillancube.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\serveur local\paper 1.16.3\plugins\untitled\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD407BD-430D-4721-8464-FD0F630F11B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92389891-1C1A-4051-9ACB-E37AE89D4048}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-75" yWindow="-75" windowWidth="28950" windowHeight="16350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>MILESTONE:</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>ban Of atro 5</t>
-  </si>
-  <si>
-    <t>KB 3</t>
   </si>
   <si>
     <t xml:space="preserve"> Stone: </t>
@@ -195,7 +192,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -214,13 +211,25 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -232,15 +241,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,7 +532,7 @@
   <dimension ref="A3:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -529,7 +541,7 @@
     <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -581,7 +593,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -607,9 +619,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -633,12 +645,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -664,85 +676,85 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="1">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3">
         <v>6</v>
       </c>
-      <c r="E12" s="1">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1">
-        <v>8</v>
-      </c>
-      <c r="G12" s="1">
+      <c r="E12" s="3">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3">
         <v>9</v>
       </c>
-      <c r="H12" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="H12" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="1">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="3">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3">
         <v>6</v>
       </c>
-      <c r="E13" s="1">
-        <v>7</v>
-      </c>
-      <c r="F13" s="1">
-        <v>8</v>
-      </c>
-      <c r="G13" s="1">
+      <c r="E13" s="3">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3">
         <v>9</v>
       </c>
-      <c r="H13" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="H13" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="1">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C14" s="3">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3">
         <v>6</v>
       </c>
-      <c r="E14" s="2">
-        <v>7</v>
-      </c>
-      <c r="F14" s="2">
-        <v>8</v>
-      </c>
-      <c r="G14" s="2">
+      <c r="E14" s="3">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3">
         <v>9</v>
       </c>
-      <c r="H14" s="2">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -794,7 +806,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -820,33 +832,33 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="3">
         <v>6</v>
       </c>
-      <c r="D18" s="1">
-        <v>7</v>
-      </c>
-      <c r="E18" s="1">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="D18" s="3">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3">
+        <v>8</v>
+      </c>
+      <c r="F18" s="3">
         <v>9</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="3">
         <v>10</v>
       </c>
-      <c r="H18" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H18" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -872,7 +884,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -929,12 +941,8 @@
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>

</xml_diff>